<commit_message>
Update with 10-28-2020 data
</commit_message>
<xml_diff>
--- a/Resources/Covid_19_Santa_Clarita_Valley.xlsx
+++ b/Resources/Covid_19_Santa_Clarita_Valley.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gitlab\Covid19\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3BD39C10-23FB-49A9-99FB-49E793BDFF11}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2AA563-FA5D-4FB9-A116-87AD9630DE4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31695" yWindow="555" windowWidth="21600" windowHeight="11385" xr2:uid="{175BF5D9-CF78-4E1F-BAF3-22C0D039EF3C}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{175BF5D9-CF78-4E1F-BAF3-22C0D039EF3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBB7B3D-0C6E-41F4-B785-3A162533B78A}">
-  <dimension ref="A1:D94"/>
+  <dimension ref="A1:D95"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="J91" sqref="J91"/>
+      <selection activeCell="D95" sqref="D95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1283,7 @@
         <v>22</v>
       </c>
       <c r="D55" s="2">
-        <f t="shared" ref="D55:D94" si="3">AVERAGE(C49:C55)</f>
+        <f t="shared" ref="D55:D95" si="3">AVERAGE(C49:C55)</f>
         <v>23</v>
       </c>
     </row>
@@ -1340,7 +1340,7 @@
         <v>5742</v>
       </c>
       <c r="C59" s="2">
-        <f t="shared" ref="C59:C94" si="4">B59-B58</f>
+        <f t="shared" ref="C59:C95" si="4">B59-B58</f>
         <v>17</v>
       </c>
       <c r="D59" s="2">
@@ -1907,6 +1907,22 @@
       <c r="D94" s="2">
         <f t="shared" si="3"/>
         <v>54.571428571428569</v>
+      </c>
+    </row>
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A95" s="3">
+        <v>44132</v>
+      </c>
+      <c r="B95">
+        <v>7071</v>
+      </c>
+      <c r="C95" s="2">
+        <f t="shared" si="4"/>
+        <v>14</v>
+      </c>
+      <c r="D95" s="2">
+        <f t="shared" si="3"/>
+        <v>54.428571428571431</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Update notebook for 10-30-2020
</commit_message>
<xml_diff>
--- a/Resources/Covid_19_Santa_Clarita_Valley.xlsx
+++ b/Resources/Covid_19_Santa_Clarita_Valley.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gitlab\Covid19\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7D2AA563-FA5D-4FB9-A116-87AD9630DE4F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896C08F3-AE62-47E8-A3E8-F57E4731C855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="780" yWindow="780" windowWidth="21600" windowHeight="11385" xr2:uid="{175BF5D9-CF78-4E1F-BAF3-22C0D039EF3C}"/>
+    <workbookView xWindow="3930" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{175BF5D9-CF78-4E1F-BAF3-22C0D039EF3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBB7B3D-0C6E-41F4-B785-3A162533B78A}">
-  <dimension ref="A1:D95"/>
+  <dimension ref="A1:D96"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D95" sqref="D95"/>
+      <selection activeCell="D97" sqref="D97"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1283,7 @@
         <v>22</v>
       </c>
       <c r="D55" s="2">
-        <f t="shared" ref="D55:D95" si="3">AVERAGE(C49:C55)</f>
+        <f t="shared" ref="D55:D96" si="3">AVERAGE(C49:C55)</f>
         <v>23</v>
       </c>
     </row>
@@ -1340,7 +1340,7 @@
         <v>5742</v>
       </c>
       <c r="C59" s="2">
-        <f t="shared" ref="C59:C95" si="4">B59-B58</f>
+        <f t="shared" ref="C59:C96" si="4">B59-B58</f>
         <v>17</v>
       </c>
       <c r="D59" s="2">
@@ -1923,6 +1923,22 @@
       <c r="D95" s="2">
         <f t="shared" si="3"/>
         <v>54.428571428571431</v>
+      </c>
+    </row>
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A96" s="3">
+        <v>44133</v>
+      </c>
+      <c r="B96">
+        <v>7170</v>
+      </c>
+      <c r="C96" s="2">
+        <f t="shared" si="4"/>
+        <v>99</v>
+      </c>
+      <c r="D96" s="2">
+        <f>AVERAGE(C90:C96)</f>
+        <v>49.714285714285715</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update data for 11-02-2020
</commit_message>
<xml_diff>
--- a/Resources/Covid_19_Santa_Clarita_Valley.xlsx
+++ b/Resources/Covid_19_Santa_Clarita_Valley.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Gitlab\Covid19\Resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{896C08F3-AE62-47E8-A3E8-F57E4731C855}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{673D2737-63CD-4FEE-B9FE-03B83D32333F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3930" yWindow="3120" windowWidth="21600" windowHeight="11385" xr2:uid="{175BF5D9-CF78-4E1F-BAF3-22C0D039EF3C}"/>
+    <workbookView xWindow="6000" yWindow="960" windowWidth="21600" windowHeight="11385" xr2:uid="{175BF5D9-CF78-4E1F-BAF3-22C0D039EF3C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -414,10 +414,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DBB7B3D-0C6E-41F4-B785-3A162533B78A}">
-  <dimension ref="A1:D96"/>
+  <dimension ref="A1:D100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
-      <selection activeCell="D97" sqref="D97"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="A99" sqref="A99:A100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1283,7 +1283,7 @@
         <v>22</v>
       </c>
       <c r="D55" s="2">
-        <f t="shared" ref="D55:D96" si="3">AVERAGE(C49:C55)</f>
+        <f t="shared" ref="D55:D95" si="3">AVERAGE(C49:C55)</f>
         <v>23</v>
       </c>
     </row>
@@ -1340,7 +1340,7 @@
         <v>5742</v>
       </c>
       <c r="C59" s="2">
-        <f t="shared" ref="C59:C96" si="4">B59-B58</f>
+        <f t="shared" ref="C59:C100" si="4">B59-B58</f>
         <v>17</v>
       </c>
       <c r="D59" s="2">
@@ -1930,15 +1930,79 @@
         <v>44133</v>
       </c>
       <c r="B96">
-        <v>7170</v>
+        <v>7121</v>
       </c>
       <c r="C96" s="2">
         <f t="shared" si="4"/>
-        <v>99</v>
+        <v>50</v>
       </c>
       <c r="D96" s="2">
         <f>AVERAGE(C90:C96)</f>
-        <v>49.714285714285715</v>
+        <v>42.714285714285715</v>
+      </c>
+    </row>
+    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A97" s="3">
+        <v>44134</v>
+      </c>
+      <c r="B97">
+        <v>7170</v>
+      </c>
+      <c r="C97" s="2">
+        <f t="shared" si="4"/>
+        <v>49</v>
+      </c>
+      <c r="D97" s="2">
+        <f>AVERAGE(C91:C97)</f>
+        <v>42.857142857142854</v>
+      </c>
+    </row>
+    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A98" s="3">
+        <v>44135</v>
+      </c>
+      <c r="B98">
+        <v>7205</v>
+      </c>
+      <c r="C98" s="2">
+        <f t="shared" si="4"/>
+        <v>35</v>
+      </c>
+      <c r="D98" s="2">
+        <f t="shared" ref="D98:D100" si="5">AVERAGE(C92:C98)</f>
+        <v>40.857142857142854</v>
+      </c>
+    </row>
+    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A99" s="3">
+        <v>44136</v>
+      </c>
+      <c r="B99">
+        <v>7241</v>
+      </c>
+      <c r="C99" s="2">
+        <f t="shared" si="4"/>
+        <v>36</v>
+      </c>
+      <c r="D99" s="2">
+        <f t="shared" si="5"/>
+        <v>39</v>
+      </c>
+    </row>
+    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A100" s="3">
+        <v>44137</v>
+      </c>
+      <c r="B100">
+        <v>7288</v>
+      </c>
+      <c r="C100" s="2">
+        <f t="shared" si="4"/>
+        <v>47</v>
+      </c>
+      <c r="D100" s="2">
+        <f t="shared" si="5"/>
+        <v>41.285714285714285</v>
       </c>
     </row>
   </sheetData>

</xml_diff>